<commit_message>
Fix PS for L1_AlwaysTrue in "EmittanceScan" column
</commit_message>
<xml_diff>
--- a/official/L1Menu_Collisions2025_v1_1_1/PrescaleTable/L1Menu_Collisions2025_v1_1_1.xlsx
+++ b/official/L1Menu_Collisions2025_v1_1_1/PrescaleTable/L1Menu_Collisions2025_v1_1_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/L1MenuRun3-May16/official/L1Menu_Collisions2025_v1_1_1/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5784389-6BF8-A846-A549-714B6A32AC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E76930-02A6-2444-A831-DE759D90DBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="760" windowWidth="27760" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1852,13 +1852,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R470"/>
+  <dimension ref="A1:R466"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A434" workbookViewId="0">
-      <selection activeCell="G442" sqref="G442"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="60.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1913,7 +1913,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1964,7 +1964,7 @@
       </c>
       <c r="R2" s="3"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2015,7 +2015,7 @@
       </c>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
       <c r="R4" s="3"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2117,7 +2117,7 @@
       </c>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2219,7 +2219,7 @@
       </c>
       <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2270,7 +2270,7 @@
       </c>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2372,7 +2372,7 @@
       </c>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2474,7 +2474,7 @@
       </c>
       <c r="R12" s="3"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2525,7 +2525,7 @@
       </c>
       <c r="R13" s="3"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2576,7 +2576,7 @@
       </c>
       <c r="R14" s="3"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2627,7 +2627,7 @@
       </c>
       <c r="R15" s="3"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2678,7 +2678,7 @@
       </c>
       <c r="R16" s="3"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="R17" s="3"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2780,7 +2780,7 @@
       </c>
       <c r="R18" s="3"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2831,7 +2831,7 @@
       </c>
       <c r="R19" s="3"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="R20" s="3"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2933,7 +2933,7 @@
       </c>
       <c r="R21" s="3"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2984,7 +2984,7 @@
       </c>
       <c r="R22" s="3"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3035,7 +3035,7 @@
       </c>
       <c r="R23" s="3"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3086,7 +3086,7 @@
       </c>
       <c r="R24" s="3"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3137,7 +3137,7 @@
       </c>
       <c r="R25" s="3"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="R26" s="3"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3239,7 +3239,7 @@
       </c>
       <c r="R27" s="3"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3290,7 +3290,7 @@
       </c>
       <c r="R28" s="3"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="R29" s="3"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3392,7 +3392,7 @@
       </c>
       <c r="R30" s="3"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="R31" s="3"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3494,7 +3494,7 @@
       </c>
       <c r="R32" s="3"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3545,7 +3545,7 @@
       </c>
       <c r="R33" s="3"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>34</v>
       </c>
@@ -3596,7 +3596,7 @@
       </c>
       <c r="R34" s="3"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>35</v>
       </c>
@@ -3647,7 +3647,7 @@
       </c>
       <c r="R35" s="3"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>36</v>
       </c>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="R36" s="3"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>37</v>
       </c>
@@ -3749,7 +3749,7 @@
       </c>
       <c r="R37" s="3"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>38</v>
       </c>
@@ -3800,7 +3800,7 @@
       </c>
       <c r="R38" s="3"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>39</v>
       </c>
@@ -3851,7 +3851,7 @@
       </c>
       <c r="R39" s="3"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>40</v>
       </c>
@@ -3902,7 +3902,7 @@
       </c>
       <c r="R40" s="3"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>41</v>
       </c>
@@ -3953,7 +3953,7 @@
       </c>
       <c r="R41" s="3"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>42</v>
       </c>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="R42" s="3"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>43</v>
       </c>
@@ -4055,7 +4055,7 @@
       </c>
       <c r="R43" s="3"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>44</v>
       </c>
@@ -4106,7 +4106,7 @@
       </c>
       <c r="R44" s="3"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>45</v>
       </c>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="R45" s="3"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>46</v>
       </c>
@@ -4208,7 +4208,7 @@
       </c>
       <c r="R46" s="3"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>47</v>
       </c>
@@ -4259,7 +4259,7 @@
       </c>
       <c r="R47" s="3"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>48</v>
       </c>
@@ -4310,7 +4310,7 @@
       </c>
       <c r="R48" s="3"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>49</v>
       </c>
@@ -4361,7 +4361,7 @@
       </c>
       <c r="R49" s="3"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>50</v>
       </c>
@@ -4412,7 +4412,7 @@
       </c>
       <c r="R50" s="3"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>51</v>
       </c>
@@ -4463,7 +4463,7 @@
       </c>
       <c r="R51" s="3"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>52</v>
       </c>
@@ -4514,7 +4514,7 @@
       </c>
       <c r="R52" s="3"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>53</v>
       </c>
@@ -4565,7 +4565,7 @@
       </c>
       <c r="R53" s="3"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>54</v>
       </c>
@@ -4616,7 +4616,7 @@
       </c>
       <c r="R54" s="3"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>56</v>
       </c>
@@ -4667,7 +4667,7 @@
       </c>
       <c r="R55" s="3"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>57</v>
       </c>
@@ -4718,7 +4718,7 @@
       </c>
       <c r="R56" s="3"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>58</v>
       </c>
@@ -4769,7 +4769,7 @@
       </c>
       <c r="R57" s="3"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>59</v>
       </c>
@@ -4820,7 +4820,7 @@
       </c>
       <c r="R58" s="3"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>60</v>
       </c>
@@ -4871,7 +4871,7 @@
       </c>
       <c r="R59" s="3"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>61</v>
       </c>
@@ -4922,7 +4922,7 @@
       </c>
       <c r="R60" s="3"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>62</v>
       </c>
@@ -4973,7 +4973,7 @@
       </c>
       <c r="R61" s="3"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>63</v>
       </c>
@@ -5024,7 +5024,7 @@
       </c>
       <c r="R62" s="3"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>64</v>
       </c>
@@ -5075,7 +5075,7 @@
       </c>
       <c r="R63" s="3"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>65</v>
       </c>
@@ -5126,7 +5126,7 @@
       </c>
       <c r="R64" s="3"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>66</v>
       </c>
@@ -5177,7 +5177,7 @@
       </c>
       <c r="R65" s="3"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>67</v>
       </c>
@@ -5228,7 +5228,7 @@
       </c>
       <c r="R66" s="3"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>68</v>
       </c>
@@ -5279,7 +5279,7 @@
       </c>
       <c r="R67" s="3"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>69</v>
       </c>
@@ -5330,7 +5330,7 @@
       </c>
       <c r="R68" s="3"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>70</v>
       </c>
@@ -5381,7 +5381,7 @@
       </c>
       <c r="R69" s="3"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>71</v>
       </c>
@@ -5432,7 +5432,7 @@
       </c>
       <c r="R70" s="3"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>72</v>
       </c>
@@ -5483,7 +5483,7 @@
       </c>
       <c r="R71" s="3"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>73</v>
       </c>
@@ -5534,7 +5534,7 @@
       </c>
       <c r="R72" s="3"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>74</v>
       </c>
@@ -5585,7 +5585,7 @@
       </c>
       <c r="R73" s="3"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>75</v>
       </c>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="R74" s="3"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>76</v>
       </c>
@@ -5687,7 +5687,7 @@
       </c>
       <c r="R75" s="3"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>78</v>
       </c>
@@ -5738,7 +5738,7 @@
       </c>
       <c r="R76" s="3"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>79</v>
       </c>
@@ -5789,7 +5789,7 @@
       </c>
       <c r="R77" s="3"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>80</v>
       </c>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="R78" s="3"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>81</v>
       </c>
@@ -5891,7 +5891,7 @@
       </c>
       <c r="R79" s="3"/>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>82</v>
       </c>
@@ -5942,7 +5942,7 @@
       </c>
       <c r="R80" s="3"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>83</v>
       </c>
@@ -5993,7 +5993,7 @@
       </c>
       <c r="R81" s="3"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>84</v>
       </c>
@@ -6044,7 +6044,7 @@
       </c>
       <c r="R82" s="3"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>85</v>
       </c>
@@ -6095,7 +6095,7 @@
       </c>
       <c r="R83" s="3"/>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>86</v>
       </c>
@@ -6146,7 +6146,7 @@
       </c>
       <c r="R84" s="3"/>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>87</v>
       </c>
@@ -6197,7 +6197,7 @@
       </c>
       <c r="R85" s="3"/>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>88</v>
       </c>
@@ -6248,7 +6248,7 @@
       </c>
       <c r="R86" s="3"/>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>89</v>
       </c>
@@ -6299,7 +6299,7 @@
       </c>
       <c r="R87" s="3"/>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>90</v>
       </c>
@@ -6350,7 +6350,7 @@
       </c>
       <c r="R88" s="3"/>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>91</v>
       </c>
@@ -6401,7 +6401,7 @@
       </c>
       <c r="R89" s="3"/>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>92</v>
       </c>
@@ -6452,7 +6452,7 @@
       </c>
       <c r="R90" s="3"/>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>93</v>
       </c>
@@ -6503,7 +6503,7 @@
       </c>
       <c r="R91" s="3"/>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>94</v>
       </c>
@@ -6554,7 +6554,7 @@
       </c>
       <c r="R92" s="3"/>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>95</v>
       </c>
@@ -6605,7 +6605,7 @@
       </c>
       <c r="R93" s="3"/>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>96</v>
       </c>
@@ -6656,7 +6656,7 @@
       </c>
       <c r="R94" s="3"/>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>97</v>
       </c>
@@ -6707,7 +6707,7 @@
       </c>
       <c r="R95" s="3"/>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>98</v>
       </c>
@@ -6758,7 +6758,7 @@
       </c>
       <c r="R96" s="3"/>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>99</v>
       </c>
@@ -6809,7 +6809,7 @@
       </c>
       <c r="R97" s="3"/>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>100</v>
       </c>
@@ -6860,7 +6860,7 @@
       </c>
       <c r="R98" s="3"/>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>101</v>
       </c>
@@ -6911,7 +6911,7 @@
       </c>
       <c r="R99" s="3"/>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>102</v>
       </c>
@@ -6962,7 +6962,7 @@
       </c>
       <c r="R100" s="3"/>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>103</v>
       </c>
@@ -7013,7 +7013,7 @@
       </c>
       <c r="R101" s="3"/>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>104</v>
       </c>
@@ -7064,7 +7064,7 @@
       </c>
       <c r="R102" s="3"/>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>105</v>
       </c>
@@ -7115,7 +7115,7 @@
       </c>
       <c r="R103" s="3"/>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>106</v>
       </c>
@@ -7166,7 +7166,7 @@
       </c>
       <c r="R104" s="3"/>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>107</v>
       </c>
@@ -7217,7 +7217,7 @@
       </c>
       <c r="R105" s="3"/>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>108</v>
       </c>
@@ -7268,7 +7268,7 @@
       </c>
       <c r="R106" s="3"/>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>109</v>
       </c>
@@ -7319,7 +7319,7 @@
       </c>
       <c r="R107" s="3"/>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>110</v>
       </c>
@@ -7370,7 +7370,7 @@
       </c>
       <c r="R108" s="3"/>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>111</v>
       </c>
@@ -7421,7 +7421,7 @@
       </c>
       <c r="R109" s="3"/>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>112</v>
       </c>
@@ -7472,7 +7472,7 @@
       </c>
       <c r="R110" s="3"/>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>113</v>
       </c>
@@ -7523,7 +7523,7 @@
       </c>
       <c r="R111" s="3"/>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>114</v>
       </c>
@@ -7574,7 +7574,7 @@
       </c>
       <c r="R112" s="3"/>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>115</v>
       </c>
@@ -7625,7 +7625,7 @@
       </c>
       <c r="R113" s="3"/>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>116</v>
       </c>
@@ -7676,7 +7676,7 @@
       </c>
       <c r="R114" s="3"/>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>117</v>
       </c>
@@ -7727,7 +7727,7 @@
       </c>
       <c r="R115" s="3"/>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>118</v>
       </c>
@@ -7778,7 +7778,7 @@
       </c>
       <c r="R116" s="3"/>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>119</v>
       </c>
@@ -7829,7 +7829,7 @@
       </c>
       <c r="R117" s="3"/>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>120</v>
       </c>
@@ -7880,7 +7880,7 @@
       </c>
       <c r="R118" s="3"/>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>121</v>
       </c>
@@ -7931,7 +7931,7 @@
       </c>
       <c r="R119" s="3"/>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>122</v>
       </c>
@@ -7982,7 +7982,7 @@
       </c>
       <c r="R120" s="3"/>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>123</v>
       </c>
@@ -8033,7 +8033,7 @@
       </c>
       <c r="R121" s="3"/>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>124</v>
       </c>
@@ -8084,7 +8084,7 @@
       </c>
       <c r="R122" s="3"/>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>125</v>
       </c>
@@ -8135,7 +8135,7 @@
       </c>
       <c r="R123" s="3"/>
     </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>126</v>
       </c>
@@ -8186,7 +8186,7 @@
       </c>
       <c r="R124" s="3"/>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>127</v>
       </c>
@@ -8237,7 +8237,7 @@
       </c>
       <c r="R125" s="3"/>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>128</v>
       </c>
@@ -8288,7 +8288,7 @@
       </c>
       <c r="R126" s="3"/>
     </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>129</v>
       </c>
@@ -8339,7 +8339,7 @@
       </c>
       <c r="R127" s="3"/>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>130</v>
       </c>
@@ -8390,7 +8390,7 @@
       </c>
       <c r="R128" s="3"/>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>131</v>
       </c>
@@ -8441,7 +8441,7 @@
       </c>
       <c r="R129" s="3"/>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>132</v>
       </c>
@@ -8492,7 +8492,7 @@
       </c>
       <c r="R130" s="3"/>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>133</v>
       </c>
@@ -8543,7 +8543,7 @@
       </c>
       <c r="R131" s="3"/>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>134</v>
       </c>
@@ -8594,7 +8594,7 @@
       </c>
       <c r="R132" s="3"/>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>135</v>
       </c>
@@ -8645,7 +8645,7 @@
       </c>
       <c r="R133" s="3"/>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>136</v>
       </c>
@@ -8696,7 +8696,7 @@
       </c>
       <c r="R134" s="3"/>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>137</v>
       </c>
@@ -8747,7 +8747,7 @@
       </c>
       <c r="R135" s="3"/>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>138</v>
       </c>
@@ -8798,7 +8798,7 @@
       </c>
       <c r="R136" s="3"/>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>139</v>
       </c>
@@ -8849,7 +8849,7 @@
       </c>
       <c r="R137" s="3"/>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>140</v>
       </c>
@@ -8900,7 +8900,7 @@
       </c>
       <c r="R138" s="3"/>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>141</v>
       </c>
@@ -8951,7 +8951,7 @@
       </c>
       <c r="R139" s="3"/>
     </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>142</v>
       </c>
@@ -9002,7 +9002,7 @@
       </c>
       <c r="R140" s="3"/>
     </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>143</v>
       </c>
@@ -9053,7 +9053,7 @@
       </c>
       <c r="R141" s="3"/>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>144</v>
       </c>
@@ -9104,7 +9104,7 @@
       </c>
       <c r="R142" s="3"/>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>145</v>
       </c>
@@ -9155,7 +9155,7 @@
       </c>
       <c r="R143" s="3"/>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>146</v>
       </c>
@@ -9206,7 +9206,7 @@
       </c>
       <c r="R144" s="3"/>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>147</v>
       </c>
@@ -9257,7 +9257,7 @@
       </c>
       <c r="R145" s="3"/>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>148</v>
       </c>
@@ -9308,7 +9308,7 @@
       </c>
       <c r="R146" s="3"/>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>149</v>
       </c>
@@ -9359,7 +9359,7 @@
       </c>
       <c r="R147" s="3"/>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>150</v>
       </c>
@@ -9410,7 +9410,7 @@
       </c>
       <c r="R148" s="3"/>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>151</v>
       </c>
@@ -9461,7 +9461,7 @@
       </c>
       <c r="R149" s="3"/>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>152</v>
       </c>
@@ -9512,7 +9512,7 @@
       </c>
       <c r="R150" s="3"/>
     </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>153</v>
       </c>
@@ -9563,7 +9563,7 @@
       </c>
       <c r="R151" s="3"/>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>154</v>
       </c>
@@ -9614,7 +9614,7 @@
       </c>
       <c r="R152" s="3"/>
     </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>155</v>
       </c>
@@ -9665,7 +9665,7 @@
       </c>
       <c r="R153" s="3"/>
     </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>156</v>
       </c>
@@ -9716,7 +9716,7 @@
       </c>
       <c r="R154" s="3"/>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>157</v>
       </c>
@@ -9767,7 +9767,7 @@
       </c>
       <c r="R155" s="3"/>
     </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>158</v>
       </c>
@@ -9818,7 +9818,7 @@
       </c>
       <c r="R156" s="3"/>
     </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>159</v>
       </c>
@@ -9869,7 +9869,7 @@
       </c>
       <c r="R157" s="3"/>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>160</v>
       </c>
@@ -9920,7 +9920,7 @@
       </c>
       <c r="R158" s="3"/>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>161</v>
       </c>
@@ -9971,7 +9971,7 @@
       </c>
       <c r="R159" s="3"/>
     </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>162</v>
       </c>
@@ -10022,7 +10022,7 @@
       </c>
       <c r="R160" s="3"/>
     </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>163</v>
       </c>
@@ -10073,7 +10073,7 @@
       </c>
       <c r="R161" s="3"/>
     </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>164</v>
       </c>
@@ -10124,7 +10124,7 @@
       </c>
       <c r="R162" s="3"/>
     </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>173</v>
       </c>
@@ -10175,7 +10175,7 @@
       </c>
       <c r="R163" s="3"/>
     </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>174</v>
       </c>
@@ -10226,7 +10226,7 @@
       </c>
       <c r="R164" s="3"/>
     </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>175</v>
       </c>
@@ -10277,7 +10277,7 @@
       </c>
       <c r="R165" s="3"/>
     </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>176</v>
       </c>
@@ -10328,7 +10328,7 @@
       </c>
       <c r="R166" s="3"/>
     </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>177</v>
       </c>
@@ -10379,7 +10379,7 @@
       </c>
       <c r="R167" s="3"/>
     </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>178</v>
       </c>
@@ -10430,7 +10430,7 @@
       </c>
       <c r="R168" s="3"/>
     </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>179</v>
       </c>
@@ -10481,7 +10481,7 @@
       </c>
       <c r="R169" s="3"/>
     </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>180</v>
       </c>
@@ -10532,7 +10532,7 @@
       </c>
       <c r="R170" s="3"/>
     </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>181</v>
       </c>
@@ -10583,7 +10583,7 @@
       </c>
       <c r="R171" s="3"/>
     </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>182</v>
       </c>
@@ -10634,7 +10634,7 @@
       </c>
       <c r="R172" s="3"/>
     </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>183</v>
       </c>
@@ -10685,7 +10685,7 @@
       </c>
       <c r="R173" s="3"/>
     </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>184</v>
       </c>
@@ -10736,7 +10736,7 @@
       </c>
       <c r="R174" s="3"/>
     </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>185</v>
       </c>
@@ -10787,7 +10787,7 @@
       </c>
       <c r="R175" s="3"/>
     </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>186</v>
       </c>
@@ -10838,7 +10838,7 @@
       </c>
       <c r="R176" s="3"/>
     </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>187</v>
       </c>
@@ -10889,7 +10889,7 @@
       </c>
       <c r="R177" s="3"/>
     </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>188</v>
       </c>
@@ -10940,7 +10940,7 @@
       </c>
       <c r="R178" s="3"/>
     </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>189</v>
       </c>
@@ -10991,7 +10991,7 @@
       </c>
       <c r="R179" s="3"/>
     </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>190</v>
       </c>
@@ -11042,7 +11042,7 @@
       </c>
       <c r="R180" s="3"/>
     </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>191</v>
       </c>
@@ -11093,7 +11093,7 @@
       </c>
       <c r="R181" s="3"/>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>192</v>
       </c>
@@ -11144,7 +11144,7 @@
       </c>
       <c r="R182" s="3"/>
     </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>193</v>
       </c>
@@ -11195,7 +11195,7 @@
       </c>
       <c r="R183" s="3"/>
     </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>194</v>
       </c>
@@ -11246,7 +11246,7 @@
       </c>
       <c r="R184" s="3"/>
     </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>195</v>
       </c>
@@ -11297,7 +11297,7 @@
       </c>
       <c r="R185" s="3"/>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>196</v>
       </c>
@@ -11348,7 +11348,7 @@
       </c>
       <c r="R186" s="3"/>
     </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>197</v>
       </c>
@@ -11399,7 +11399,7 @@
       </c>
       <c r="R187" s="3"/>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>198</v>
       </c>
@@ -11450,7 +11450,7 @@
       </c>
       <c r="R188" s="3"/>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>199</v>
       </c>
@@ -11501,7 +11501,7 @@
       </c>
       <c r="R189" s="3"/>
     </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>200</v>
       </c>
@@ -11552,7 +11552,7 @@
       </c>
       <c r="R190" s="3"/>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>201</v>
       </c>
@@ -11603,7 +11603,7 @@
       </c>
       <c r="R191" s="3"/>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>202</v>
       </c>
@@ -11654,7 +11654,7 @@
       </c>
       <c r="R192" s="3"/>
     </row>
-    <row r="193" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>203</v>
       </c>
@@ -11705,7 +11705,7 @@
       </c>
       <c r="R193" s="3"/>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>204</v>
       </c>
@@ -11756,7 +11756,7 @@
       </c>
       <c r="R194" s="3"/>
     </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>205</v>
       </c>
@@ -11807,7 +11807,7 @@
       </c>
       <c r="R195" s="3"/>
     </row>
-    <row r="196" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>206</v>
       </c>
@@ -11858,7 +11858,7 @@
       </c>
       <c r="R196" s="3"/>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>207</v>
       </c>
@@ -11909,7 +11909,7 @@
       </c>
       <c r="R197" s="3"/>
     </row>
-    <row r="198" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>208</v>
       </c>
@@ -11960,7 +11960,7 @@
       </c>
       <c r="R198" s="3"/>
     </row>
-    <row r="199" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>209</v>
       </c>
@@ -12011,7 +12011,7 @@
       </c>
       <c r="R199" s="3"/>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>210</v>
       </c>
@@ -12062,7 +12062,7 @@
       </c>
       <c r="R200" s="3"/>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>211</v>
       </c>
@@ -12113,7 +12113,7 @@
       </c>
       <c r="R201" s="3"/>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>212</v>
       </c>
@@ -12164,7 +12164,7 @@
       </c>
       <c r="R202" s="3"/>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>213</v>
       </c>
@@ -12215,7 +12215,7 @@
       </c>
       <c r="R203" s="3"/>
     </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>214</v>
       </c>
@@ -12266,7 +12266,7 @@
       </c>
       <c r="R204" s="3"/>
     </row>
-    <row r="205" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>215</v>
       </c>
@@ -12317,7 +12317,7 @@
       </c>
       <c r="R205" s="3"/>
     </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>216</v>
       </c>
@@ -12368,7 +12368,7 @@
       </c>
       <c r="R206" s="3"/>
     </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>217</v>
       </c>
@@ -12419,7 +12419,7 @@
       </c>
       <c r="R207" s="3"/>
     </row>
-    <row r="208" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>218</v>
       </c>
@@ -12470,7 +12470,7 @@
       </c>
       <c r="R208" s="3"/>
     </row>
-    <row r="209" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>220</v>
       </c>
@@ -12521,7 +12521,7 @@
       </c>
       <c r="R209" s="3"/>
     </row>
-    <row r="210" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>221</v>
       </c>
@@ -12572,7 +12572,7 @@
       </c>
       <c r="R210" s="3"/>
     </row>
-    <row r="211" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>222</v>
       </c>
@@ -12623,7 +12623,7 @@
       </c>
       <c r="R211" s="3"/>
     </row>
-    <row r="212" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>223</v>
       </c>
@@ -12674,7 +12674,7 @@
       </c>
       <c r="R212" s="3"/>
     </row>
-    <row r="213" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>224</v>
       </c>
@@ -12725,7 +12725,7 @@
       </c>
       <c r="R213" s="3"/>
     </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>225</v>
       </c>
@@ -12776,7 +12776,7 @@
       </c>
       <c r="R214" s="3"/>
     </row>
-    <row r="215" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>226</v>
       </c>
@@ -12827,7 +12827,7 @@
       </c>
       <c r="R215" s="3"/>
     </row>
-    <row r="216" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>227</v>
       </c>
@@ -12878,7 +12878,7 @@
       </c>
       <c r="R216" s="3"/>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>228</v>
       </c>
@@ -12929,7 +12929,7 @@
       </c>
       <c r="R217" s="3"/>
     </row>
-    <row r="218" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>229</v>
       </c>
@@ -12980,7 +12980,7 @@
       </c>
       <c r="R218" s="3"/>
     </row>
-    <row r="219" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>230</v>
       </c>
@@ -13031,7 +13031,7 @@
       </c>
       <c r="R219" s="3"/>
     </row>
-    <row r="220" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>231</v>
       </c>
@@ -13082,7 +13082,7 @@
       </c>
       <c r="R220" s="3"/>
     </row>
-    <row r="221" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>232</v>
       </c>
@@ -13133,7 +13133,7 @@
       </c>
       <c r="R221" s="3"/>
     </row>
-    <row r="222" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>233</v>
       </c>
@@ -13184,7 +13184,7 @@
       </c>
       <c r="R222" s="3"/>
     </row>
-    <row r="223" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>234</v>
       </c>
@@ -13235,7 +13235,7 @@
       </c>
       <c r="R223" s="3"/>
     </row>
-    <row r="224" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>235</v>
       </c>
@@ -13286,7 +13286,7 @@
       </c>
       <c r="R224" s="3"/>
     </row>
-    <row r="225" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>236</v>
       </c>
@@ -13337,7 +13337,7 @@
       </c>
       <c r="R225" s="3"/>
     </row>
-    <row r="226" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>237</v>
       </c>
@@ -13388,7 +13388,7 @@
       </c>
       <c r="R226" s="3"/>
     </row>
-    <row r="227" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>238</v>
       </c>
@@ -13439,7 +13439,7 @@
       </c>
       <c r="R227" s="3"/>
     </row>
-    <row r="228" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>239</v>
       </c>
@@ -13490,7 +13490,7 @@
       </c>
       <c r="R228" s="3"/>
     </row>
-    <row r="229" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>240</v>
       </c>
@@ -13541,7 +13541,7 @@
       </c>
       <c r="R229" s="3"/>
     </row>
-    <row r="230" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>241</v>
       </c>
@@ -13592,7 +13592,7 @@
       </c>
       <c r="R230" s="3"/>
     </row>
-    <row r="231" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>242</v>
       </c>
@@ -13643,7 +13643,7 @@
       </c>
       <c r="R231" s="3"/>
     </row>
-    <row r="232" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>248</v>
       </c>
@@ -13694,7 +13694,7 @@
       </c>
       <c r="R232" s="3"/>
     </row>
-    <row r="233" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>249</v>
       </c>
@@ -13745,7 +13745,7 @@
       </c>
       <c r="R233" s="3"/>
     </row>
-    <row r="234" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>250</v>
       </c>
@@ -13796,7 +13796,7 @@
       </c>
       <c r="R234" s="3"/>
     </row>
-    <row r="235" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>257</v>
       </c>
@@ -13847,7 +13847,7 @@
       </c>
       <c r="R235" s="3"/>
     </row>
-    <row r="236" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>258</v>
       </c>
@@ -13898,7 +13898,7 @@
       </c>
       <c r="R236" s="3"/>
     </row>
-    <row r="237" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>259</v>
       </c>
@@ -13949,7 +13949,7 @@
       </c>
       <c r="R237" s="3"/>
     </row>
-    <row r="238" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>263</v>
       </c>
@@ -14000,7 +14000,7 @@
       </c>
       <c r="R238" s="3"/>
     </row>
-    <row r="239" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>264</v>
       </c>
@@ -14051,7 +14051,7 @@
       </c>
       <c r="R239" s="3"/>
     </row>
-    <row r="240" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>266</v>
       </c>
@@ -14102,7 +14102,7 @@
       </c>
       <c r="R240" s="3"/>
     </row>
-    <row r="241" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>267</v>
       </c>
@@ -14153,7 +14153,7 @@
       </c>
       <c r="R241" s="3"/>
     </row>
-    <row r="242" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>268</v>
       </c>
@@ -14204,7 +14204,7 @@
       </c>
       <c r="R242" s="3"/>
     </row>
-    <row r="243" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>269</v>
       </c>
@@ -14255,7 +14255,7 @@
       </c>
       <c r="R243" s="3"/>
     </row>
-    <row r="244" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>270</v>
       </c>
@@ -14306,7 +14306,7 @@
       </c>
       <c r="R244" s="3"/>
     </row>
-    <row r="245" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>271</v>
       </c>
@@ -14357,7 +14357,7 @@
       </c>
       <c r="R245" s="3"/>
     </row>
-    <row r="246" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>272</v>
       </c>
@@ -14408,7 +14408,7 @@
       </c>
       <c r="R246" s="3"/>
     </row>
-    <row r="247" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>273</v>
       </c>
@@ -14459,7 +14459,7 @@
       </c>
       <c r="R247" s="3"/>
     </row>
-    <row r="248" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>274</v>
       </c>
@@ -14510,7 +14510,7 @@
       </c>
       <c r="R248" s="3"/>
     </row>
-    <row r="249" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>275</v>
       </c>
@@ -14561,7 +14561,7 @@
       </c>
       <c r="R249" s="3"/>
     </row>
-    <row r="250" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>276</v>
       </c>
@@ -14612,7 +14612,7 @@
       </c>
       <c r="R250" s="3"/>
     </row>
-    <row r="251" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>277</v>
       </c>
@@ -14663,7 +14663,7 @@
       </c>
       <c r="R251" s="3"/>
     </row>
-    <row r="252" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>278</v>
       </c>
@@ -14714,7 +14714,7 @@
       </c>
       <c r="R252" s="3"/>
     </row>
-    <row r="253" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>279</v>
       </c>
@@ -14765,7 +14765,7 @@
       </c>
       <c r="R253" s="3"/>
     </row>
-    <row r="254" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>280</v>
       </c>
@@ -14816,7 +14816,7 @@
       </c>
       <c r="R254" s="3"/>
     </row>
-    <row r="255" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>281</v>
       </c>
@@ -14867,7 +14867,7 @@
       </c>
       <c r="R255" s="3"/>
     </row>
-    <row r="256" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>282</v>
       </c>
@@ -14918,7 +14918,7 @@
       </c>
       <c r="R256" s="3"/>
     </row>
-    <row r="257" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>286</v>
       </c>
@@ -14969,7 +14969,7 @@
       </c>
       <c r="R257" s="3"/>
     </row>
-    <row r="258" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>287</v>
       </c>
@@ -15020,7 +15020,7 @@
       </c>
       <c r="R258" s="3"/>
     </row>
-    <row r="259" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>288</v>
       </c>
@@ -15071,7 +15071,7 @@
       </c>
       <c r="R259" s="3"/>
     </row>
-    <row r="260" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>290</v>
       </c>
@@ -15122,7 +15122,7 @@
       </c>
       <c r="R260" s="3"/>
     </row>
-    <row r="261" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>291</v>
       </c>
@@ -15173,7 +15173,7 @@
       </c>
       <c r="R261" s="3"/>
     </row>
-    <row r="262" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>292</v>
       </c>
@@ -15224,7 +15224,7 @@
       </c>
       <c r="R262" s="3"/>
     </row>
-    <row r="263" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>296</v>
       </c>
@@ -15275,7 +15275,7 @@
       </c>
       <c r="R263" s="3"/>
     </row>
-    <row r="264" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>297</v>
       </c>
@@ -15326,7 +15326,7 @@
       </c>
       <c r="R264" s="3"/>
     </row>
-    <row r="265" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>298</v>
       </c>
@@ -15377,7 +15377,7 @@
       </c>
       <c r="R265" s="3"/>
     </row>
-    <row r="266" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>299</v>
       </c>
@@ -15428,7 +15428,7 @@
       </c>
       <c r="R266" s="3"/>
     </row>
-    <row r="267" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>300</v>
       </c>
@@ -15479,7 +15479,7 @@
       </c>
       <c r="R267" s="3"/>
     </row>
-    <row r="268" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>301</v>
       </c>
@@ -15530,7 +15530,7 @@
       </c>
       <c r="R268" s="3"/>
     </row>
-    <row r="269" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>302</v>
       </c>
@@ -15581,7 +15581,7 @@
       </c>
       <c r="R269" s="3"/>
     </row>
-    <row r="270" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>303</v>
       </c>
@@ -15632,7 +15632,7 @@
       </c>
       <c r="R270" s="3"/>
     </row>
-    <row r="271" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>304</v>
       </c>
@@ -15683,7 +15683,7 @@
       </c>
       <c r="R271" s="3"/>
     </row>
-    <row r="272" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>305</v>
       </c>
@@ -15734,7 +15734,7 @@
       </c>
       <c r="R272" s="3"/>
     </row>
-    <row r="273" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>306</v>
       </c>
@@ -15785,7 +15785,7 @@
       </c>
       <c r="R273" s="3"/>
     </row>
-    <row r="274" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>307</v>
       </c>
@@ -15836,7 +15836,7 @@
       </c>
       <c r="R274" s="3"/>
     </row>
-    <row r="275" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>308</v>
       </c>
@@ -15887,7 +15887,7 @@
       </c>
       <c r="R275" s="3"/>
     </row>
-    <row r="276" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>309</v>
       </c>
@@ -15938,7 +15938,7 @@
       </c>
       <c r="R276" s="3"/>
     </row>
-    <row r="277" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>310</v>
       </c>
@@ -15989,7 +15989,7 @@
       </c>
       <c r="R277" s="3"/>
     </row>
-    <row r="278" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>311</v>
       </c>
@@ -16040,7 +16040,7 @@
       </c>
       <c r="R278" s="3"/>
     </row>
-    <row r="279" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>312</v>
       </c>
@@ -16091,7 +16091,7 @@
       </c>
       <c r="R279" s="3"/>
     </row>
-    <row r="280" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>313</v>
       </c>
@@ -16142,7 +16142,7 @@
       </c>
       <c r="R280" s="3"/>
     </row>
-    <row r="281" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>314</v>
       </c>
@@ -16193,7 +16193,7 @@
       </c>
       <c r="R281" s="3"/>
     </row>
-    <row r="282" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>315</v>
       </c>
@@ -16244,7 +16244,7 @@
       </c>
       <c r="R282" s="3"/>
     </row>
-    <row r="283" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>316</v>
       </c>
@@ -16295,7 +16295,7 @@
       </c>
       <c r="R283" s="3"/>
     </row>
-    <row r="284" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>317</v>
       </c>
@@ -16346,7 +16346,7 @@
       </c>
       <c r="R284" s="3"/>
     </row>
-    <row r="285" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>318</v>
       </c>
@@ -16397,7 +16397,7 @@
       </c>
       <c r="R285" s="3"/>
     </row>
-    <row r="286" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>319</v>
       </c>
@@ -16448,7 +16448,7 @@
       </c>
       <c r="R286" s="3"/>
     </row>
-    <row r="287" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>320</v>
       </c>
@@ -16499,7 +16499,7 @@
       </c>
       <c r="R287" s="3"/>
     </row>
-    <row r="288" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>321</v>
       </c>
@@ -16550,7 +16550,7 @@
       </c>
       <c r="R288" s="3"/>
     </row>
-    <row r="289" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>328</v>
       </c>
@@ -16601,7 +16601,7 @@
       </c>
       <c r="R289" s="3"/>
     </row>
-    <row r="290" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>329</v>
       </c>
@@ -16652,7 +16652,7 @@
       </c>
       <c r="R290" s="3"/>
     </row>
-    <row r="291" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>330</v>
       </c>
@@ -16703,7 +16703,7 @@
       </c>
       <c r="R291" s="3"/>
     </row>
-    <row r="292" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>331</v>
       </c>
@@ -16754,7 +16754,7 @@
       </c>
       <c r="R292" s="3"/>
     </row>
-    <row r="293" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>336</v>
       </c>
@@ -16805,7 +16805,7 @@
       </c>
       <c r="R293" s="3"/>
     </row>
-    <row r="294" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>337</v>
       </c>
@@ -16856,7 +16856,7 @@
       </c>
       <c r="R294" s="3"/>
     </row>
-    <row r="295" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>338</v>
       </c>
@@ -16907,7 +16907,7 @@
       </c>
       <c r="R295" s="3"/>
     </row>
-    <row r="296" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>339</v>
       </c>
@@ -16958,7 +16958,7 @@
       </c>
       <c r="R296" s="3"/>
     </row>
-    <row r="297" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>340</v>
       </c>
@@ -17009,7 +17009,7 @@
       </c>
       <c r="R297" s="3"/>
     </row>
-    <row r="298" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>341</v>
       </c>
@@ -17060,7 +17060,7 @@
       </c>
       <c r="R298" s="3"/>
     </row>
-    <row r="299" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>342</v>
       </c>
@@ -17111,7 +17111,7 @@
       </c>
       <c r="R299" s="3"/>
     </row>
-    <row r="300" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>343</v>
       </c>
@@ -17162,7 +17162,7 @@
       </c>
       <c r="R300" s="3"/>
     </row>
-    <row r="301" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>344</v>
       </c>
@@ -17213,7 +17213,7 @@
       </c>
       <c r="R301" s="3"/>
     </row>
-    <row r="302" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>345</v>
       </c>
@@ -17264,7 +17264,7 @@
       </c>
       <c r="R302" s="3"/>
     </row>
-    <row r="303" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>346</v>
       </c>
@@ -17315,7 +17315,7 @@
       </c>
       <c r="R303" s="3"/>
     </row>
-    <row r="304" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>347</v>
       </c>
@@ -17366,7 +17366,7 @@
       </c>
       <c r="R304" s="3"/>
     </row>
-    <row r="305" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>348</v>
       </c>
@@ -17417,7 +17417,7 @@
       </c>
       <c r="R305" s="3"/>
     </row>
-    <row r="306" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>349</v>
       </c>
@@ -17468,7 +17468,7 @@
       </c>
       <c r="R306" s="3"/>
     </row>
-    <row r="307" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>350</v>
       </c>
@@ -17519,7 +17519,7 @@
       </c>
       <c r="R307" s="3"/>
     </row>
-    <row r="308" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>351</v>
       </c>
@@ -17570,7 +17570,7 @@
       </c>
       <c r="R308" s="3"/>
     </row>
-    <row r="309" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>352</v>
       </c>
@@ -17621,7 +17621,7 @@
       </c>
       <c r="R309" s="3"/>
     </row>
-    <row r="310" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>353</v>
       </c>
@@ -17672,7 +17672,7 @@
       </c>
       <c r="R310" s="3"/>
     </row>
-    <row r="311" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>354</v>
       </c>
@@ -17723,7 +17723,7 @@
       </c>
       <c r="R311" s="3"/>
     </row>
-    <row r="312" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>355</v>
       </c>
@@ -17774,7 +17774,7 @@
       </c>
       <c r="R312" s="3"/>
     </row>
-    <row r="313" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>356</v>
       </c>
@@ -17825,7 +17825,7 @@
       </c>
       <c r="R313" s="3"/>
     </row>
-    <row r="314" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>357</v>
       </c>
@@ -17876,7 +17876,7 @@
       </c>
       <c r="R314" s="3"/>
     </row>
-    <row r="315" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>358</v>
       </c>
@@ -17927,7 +17927,7 @@
       </c>
       <c r="R315" s="3"/>
     </row>
-    <row r="316" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>359</v>
       </c>
@@ -17978,7 +17978,7 @@
       </c>
       <c r="R316" s="3"/>
     </row>
-    <row r="317" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>360</v>
       </c>
@@ -18029,7 +18029,7 @@
       </c>
       <c r="R317" s="3"/>
     </row>
-    <row r="318" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>361</v>
       </c>
@@ -18080,7 +18080,7 @@
       </c>
       <c r="R318" s="3"/>
     </row>
-    <row r="319" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>362</v>
       </c>
@@ -18131,7 +18131,7 @@
       </c>
       <c r="R319" s="3"/>
     </row>
-    <row r="320" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>363</v>
       </c>
@@ -18182,7 +18182,7 @@
       </c>
       <c r="R320" s="3"/>
     </row>
-    <row r="321" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>364</v>
       </c>
@@ -18233,7 +18233,7 @@
       </c>
       <c r="R321" s="3"/>
     </row>
-    <row r="322" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>365</v>
       </c>
@@ -18284,7 +18284,7 @@
       </c>
       <c r="R322" s="3"/>
     </row>
-    <row r="323" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>366</v>
       </c>
@@ -18335,7 +18335,7 @@
       </c>
       <c r="R323" s="3"/>
     </row>
-    <row r="324" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>367</v>
       </c>
@@ -18386,7 +18386,7 @@
       </c>
       <c r="R324" s="3"/>
     </row>
-    <row r="325" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>368</v>
       </c>
@@ -18437,7 +18437,7 @@
       </c>
       <c r="R325" s="3"/>
     </row>
-    <row r="326" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>369</v>
       </c>
@@ -18488,7 +18488,7 @@
       </c>
       <c r="R326" s="3"/>
     </row>
-    <row r="327" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>370</v>
       </c>
@@ -18539,7 +18539,7 @@
       </c>
       <c r="R327" s="3"/>
     </row>
-    <row r="328" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>371</v>
       </c>
@@ -18590,7 +18590,7 @@
       </c>
       <c r="R328" s="3"/>
     </row>
-    <row r="329" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>372</v>
       </c>
@@ -18641,7 +18641,7 @@
       </c>
       <c r="R329" s="3"/>
     </row>
-    <row r="330" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>373</v>
       </c>
@@ -18692,7 +18692,7 @@
       </c>
       <c r="R330" s="3"/>
     </row>
-    <row r="331" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>374</v>
       </c>
@@ -18743,7 +18743,7 @@
       </c>
       <c r="R331" s="3"/>
     </row>
-    <row r="332" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>375</v>
       </c>
@@ -18794,7 +18794,7 @@
       </c>
       <c r="R332" s="3"/>
     </row>
-    <row r="333" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>376</v>
       </c>
@@ -18845,7 +18845,7 @@
       </c>
       <c r="R333" s="3"/>
     </row>
-    <row r="334" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>377</v>
       </c>
@@ -18896,7 +18896,7 @@
       </c>
       <c r="R334" s="3"/>
     </row>
-    <row r="335" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>378</v>
       </c>
@@ -18947,7 +18947,7 @@
       </c>
       <c r="R335" s="3"/>
     </row>
-    <row r="336" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>379</v>
       </c>
@@ -18998,7 +18998,7 @@
       </c>
       <c r="R336" s="3"/>
     </row>
-    <row r="337" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>380</v>
       </c>
@@ -19049,7 +19049,7 @@
       </c>
       <c r="R337" s="3"/>
     </row>
-    <row r="338" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>381</v>
       </c>
@@ -19100,7 +19100,7 @@
       </c>
       <c r="R338" s="3"/>
     </row>
-    <row r="339" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>382</v>
       </c>
@@ -19151,7 +19151,7 @@
       </c>
       <c r="R339" s="3"/>
     </row>
-    <row r="340" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>383</v>
       </c>
@@ -19202,7 +19202,7 @@
       </c>
       <c r="R340" s="3"/>
     </row>
-    <row r="341" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>384</v>
       </c>
@@ -19253,7 +19253,7 @@
       </c>
       <c r="R341" s="3"/>
     </row>
-    <row r="342" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>385</v>
       </c>
@@ -19304,7 +19304,7 @@
       </c>
       <c r="R342" s="3"/>
     </row>
-    <row r="343" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>386</v>
       </c>
@@ -19355,7 +19355,7 @@
       </c>
       <c r="R343" s="3"/>
     </row>
-    <row r="344" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>387</v>
       </c>
@@ -19406,7 +19406,7 @@
       </c>
       <c r="R344" s="3"/>
     </row>
-    <row r="345" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>388</v>
       </c>
@@ -19457,7 +19457,7 @@
       </c>
       <c r="R345" s="3"/>
     </row>
-    <row r="346" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>389</v>
       </c>
@@ -19508,7 +19508,7 @@
       </c>
       <c r="R346" s="3"/>
     </row>
-    <row r="347" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>390</v>
       </c>
@@ -19559,7 +19559,7 @@
       </c>
       <c r="R347" s="3"/>
     </row>
-    <row r="348" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A348">
         <v>391</v>
       </c>
@@ -19610,7 +19610,7 @@
       </c>
       <c r="R348" s="3"/>
     </row>
-    <row r="349" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>392</v>
       </c>
@@ -19661,7 +19661,7 @@
       </c>
       <c r="R349" s="3"/>
     </row>
-    <row r="350" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A350">
         <v>393</v>
       </c>
@@ -19712,7 +19712,7 @@
       </c>
       <c r="R350" s="3"/>
     </row>
-    <row r="351" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A351">
         <v>394</v>
       </c>
@@ -19763,7 +19763,7 @@
       </c>
       <c r="R351" s="3"/>
     </row>
-    <row r="352" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A352">
         <v>395</v>
       </c>
@@ -19814,7 +19814,7 @@
       </c>
       <c r="R352" s="3"/>
     </row>
-    <row r="353" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A353">
         <v>396</v>
       </c>
@@ -19865,7 +19865,7 @@
       </c>
       <c r="R353" s="3"/>
     </row>
-    <row r="354" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A354">
         <v>397</v>
       </c>
@@ -19916,7 +19916,7 @@
       </c>
       <c r="R354" s="3"/>
     </row>
-    <row r="355" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A355">
         <v>398</v>
       </c>
@@ -19967,7 +19967,7 @@
       </c>
       <c r="R355" s="3"/>
     </row>
-    <row r="356" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A356">
         <v>399</v>
       </c>
@@ -20018,7 +20018,7 @@
       </c>
       <c r="R356" s="3"/>
     </row>
-    <row r="357" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A357">
         <v>400</v>
       </c>
@@ -20069,7 +20069,7 @@
       </c>
       <c r="R357" s="3"/>
     </row>
-    <row r="358" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A358">
         <v>401</v>
       </c>
@@ -20120,7 +20120,7 @@
       </c>
       <c r="R358" s="3"/>
     </row>
-    <row r="359" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A359">
         <v>402</v>
       </c>
@@ -20171,7 +20171,7 @@
       </c>
       <c r="R359" s="3"/>
     </row>
-    <row r="360" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A360">
         <v>403</v>
       </c>
@@ -20222,7 +20222,7 @@
       </c>
       <c r="R360" s="3"/>
     </row>
-    <row r="361" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A361">
         <v>404</v>
       </c>
@@ -20273,7 +20273,7 @@
       </c>
       <c r="R361" s="3"/>
     </row>
-    <row r="362" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A362">
         <v>405</v>
       </c>
@@ -20324,7 +20324,7 @@
       </c>
       <c r="R362" s="3"/>
     </row>
-    <row r="363" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A363">
         <v>406</v>
       </c>
@@ -20375,7 +20375,7 @@
       </c>
       <c r="R363" s="3"/>
     </row>
-    <row r="364" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A364">
         <v>407</v>
       </c>
@@ -20426,7 +20426,7 @@
       </c>
       <c r="R364" s="3"/>
     </row>
-    <row r="365" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A365">
         <v>408</v>
       </c>
@@ -20477,7 +20477,7 @@
       </c>
       <c r="R365" s="3"/>
     </row>
-    <row r="366" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A366">
         <v>409</v>
       </c>
@@ -20528,7 +20528,7 @@
       </c>
       <c r="R366" s="3"/>
     </row>
-    <row r="367" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A367">
         <v>410</v>
       </c>
@@ -20579,7 +20579,7 @@
       </c>
       <c r="R367" s="3"/>
     </row>
-    <row r="368" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A368">
         <v>411</v>
       </c>
@@ -20630,7 +20630,7 @@
       </c>
       <c r="R368" s="3"/>
     </row>
-    <row r="369" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A369">
         <v>412</v>
       </c>
@@ -20681,7 +20681,7 @@
       </c>
       <c r="R369" s="3"/>
     </row>
-    <row r="370" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A370">
         <v>413</v>
       </c>
@@ -20732,7 +20732,7 @@
       </c>
       <c r="R370" s="3"/>
     </row>
-    <row r="371" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A371">
         <v>414</v>
       </c>
@@ -20783,7 +20783,7 @@
       </c>
       <c r="R371" s="3"/>
     </row>
-    <row r="372" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A372">
         <v>415</v>
       </c>
@@ -20834,7 +20834,7 @@
       </c>
       <c r="R372" s="3"/>
     </row>
-    <row r="373" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A373">
         <v>416</v>
       </c>
@@ -20885,7 +20885,7 @@
       </c>
       <c r="R373" s="3"/>
     </row>
-    <row r="374" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A374">
         <v>417</v>
       </c>
@@ -20936,7 +20936,7 @@
       </c>
       <c r="R374" s="3"/>
     </row>
-    <row r="375" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A375">
         <v>418</v>
       </c>
@@ -20987,7 +20987,7 @@
       </c>
       <c r="R375" s="3"/>
     </row>
-    <row r="376" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A376">
         <v>419</v>
       </c>
@@ -21038,7 +21038,7 @@
       </c>
       <c r="R376" s="3"/>
     </row>
-    <row r="377" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A377">
         <v>420</v>
       </c>
@@ -21089,7 +21089,7 @@
       </c>
       <c r="R377" s="3"/>
     </row>
-    <row r="378" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A378">
         <v>421</v>
       </c>
@@ -21140,7 +21140,7 @@
       </c>
       <c r="R378" s="3"/>
     </row>
-    <row r="379" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A379">
         <v>422</v>
       </c>
@@ -21191,7 +21191,7 @@
       </c>
       <c r="R379" s="3"/>
     </row>
-    <row r="380" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A380">
         <v>423</v>
       </c>
@@ -21242,7 +21242,7 @@
       </c>
       <c r="R380" s="3"/>
     </row>
-    <row r="381" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A381">
         <v>424</v>
       </c>
@@ -21293,7 +21293,7 @@
       </c>
       <c r="R381" s="3"/>
     </row>
-    <row r="382" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A382">
         <v>425</v>
       </c>
@@ -21344,7 +21344,7 @@
       </c>
       <c r="R382" s="3"/>
     </row>
-    <row r="383" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A383">
         <v>426</v>
       </c>
@@ -21395,7 +21395,7 @@
       </c>
       <c r="R383" s="3"/>
     </row>
-    <row r="384" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A384">
         <v>427</v>
       </c>
@@ -21446,7 +21446,7 @@
       </c>
       <c r="R384" s="3"/>
     </row>
-    <row r="385" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>428</v>
       </c>
@@ -21497,7 +21497,7 @@
       </c>
       <c r="R385" s="3"/>
     </row>
-    <row r="386" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A386">
         <v>429</v>
       </c>
@@ -21548,7 +21548,7 @@
       </c>
       <c r="R386" s="3"/>
     </row>
-    <row r="387" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A387">
         <v>430</v>
       </c>
@@ -21599,7 +21599,7 @@
       </c>
       <c r="R387" s="3"/>
     </row>
-    <row r="388" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A388">
         <v>431</v>
       </c>
@@ -21650,7 +21650,7 @@
       </c>
       <c r="R388" s="3"/>
     </row>
-    <row r="389" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A389">
         <v>432</v>
       </c>
@@ -21701,7 +21701,7 @@
       </c>
       <c r="R389" s="3"/>
     </row>
-    <row r="390" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A390">
         <v>433</v>
       </c>
@@ -21752,7 +21752,7 @@
       </c>
       <c r="R390" s="3"/>
     </row>
-    <row r="391" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A391">
         <v>434</v>
       </c>
@@ -21803,7 +21803,7 @@
       </c>
       <c r="R391" s="3"/>
     </row>
-    <row r="392" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A392">
         <v>435</v>
       </c>
@@ -21854,7 +21854,7 @@
       </c>
       <c r="R392" s="3"/>
     </row>
-    <row r="393" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A393">
         <v>436</v>
       </c>
@@ -21905,7 +21905,7 @@
       </c>
       <c r="R393" s="3"/>
     </row>
-    <row r="394" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A394">
         <v>437</v>
       </c>
@@ -21956,7 +21956,7 @@
       </c>
       <c r="R394" s="3"/>
     </row>
-    <row r="395" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A395">
         <v>438</v>
       </c>
@@ -22007,7 +22007,7 @@
       </c>
       <c r="R395" s="3"/>
     </row>
-    <row r="396" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A396">
         <v>439</v>
       </c>
@@ -22058,7 +22058,7 @@
       </c>
       <c r="R396" s="3"/>
     </row>
-    <row r="397" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A397">
         <v>440</v>
       </c>
@@ -22109,7 +22109,7 @@
       </c>
       <c r="R397" s="3"/>
     </row>
-    <row r="398" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A398">
         <v>441</v>
       </c>
@@ -22160,7 +22160,7 @@
       </c>
       <c r="R398" s="3"/>
     </row>
-    <row r="399" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A399">
         <v>442</v>
       </c>
@@ -22211,7 +22211,7 @@
       </c>
       <c r="R399" s="3"/>
     </row>
-    <row r="400" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A400">
         <v>444</v>
       </c>
@@ -22262,7 +22262,7 @@
       </c>
       <c r="R400" s="3"/>
     </row>
-    <row r="401" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A401">
         <v>445</v>
       </c>
@@ -22313,7 +22313,7 @@
       </c>
       <c r="R401" s="3"/>
     </row>
-    <row r="402" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A402">
         <v>446</v>
       </c>
@@ -22364,7 +22364,7 @@
       </c>
       <c r="R402" s="3"/>
     </row>
-    <row r="403" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A403">
         <v>447</v>
       </c>
@@ -22415,7 +22415,7 @@
       </c>
       <c r="R403" s="3"/>
     </row>
-    <row r="404" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A404">
         <v>448</v>
       </c>
@@ -22466,7 +22466,7 @@
       </c>
       <c r="R404" s="3"/>
     </row>
-    <row r="405" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A405">
         <v>449</v>
       </c>
@@ -22517,7 +22517,7 @@
       </c>
       <c r="R405" s="3"/>
     </row>
-    <row r="406" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A406">
         <v>450</v>
       </c>
@@ -22568,7 +22568,7 @@
       </c>
       <c r="R406" s="3"/>
     </row>
-    <row r="407" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A407">
         <v>451</v>
       </c>
@@ -22619,7 +22619,7 @@
       </c>
       <c r="R407" s="3"/>
     </row>
-    <row r="408" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A408">
         <v>452</v>
       </c>
@@ -22670,7 +22670,7 @@
       </c>
       <c r="R408" s="3"/>
     </row>
-    <row r="409" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A409">
         <v>453</v>
       </c>
@@ -22721,7 +22721,7 @@
       </c>
       <c r="R409" s="3"/>
     </row>
-    <row r="410" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A410">
         <v>454</v>
       </c>
@@ -22772,7 +22772,7 @@
       </c>
       <c r="R410" s="3"/>
     </row>
-    <row r="411" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A411">
         <v>455</v>
       </c>
@@ -22823,7 +22823,7 @@
       </c>
       <c r="R411" s="3"/>
     </row>
-    <row r="412" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A412">
         <v>456</v>
       </c>
@@ -22874,7 +22874,7 @@
       </c>
       <c r="R412" s="3"/>
     </row>
-    <row r="413" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A413">
         <v>457</v>
       </c>
@@ -22925,7 +22925,7 @@
       </c>
       <c r="R413" s="3"/>
     </row>
-    <row r="414" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A414">
         <v>458</v>
       </c>
@@ -22976,7 +22976,7 @@
       </c>
       <c r="R414" s="3"/>
     </row>
-    <row r="415" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A415">
         <v>459</v>
       </c>
@@ -23027,7 +23027,7 @@
       </c>
       <c r="R415" s="3"/>
     </row>
-    <row r="416" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A416">
         <v>460</v>
       </c>
@@ -23078,7 +23078,7 @@
       </c>
       <c r="R416" s="3"/>
     </row>
-    <row r="417" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A417">
         <v>461</v>
       </c>
@@ -23129,7 +23129,7 @@
       </c>
       <c r="R417" s="3"/>
     </row>
-    <row r="418" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A418">
         <v>462</v>
       </c>
@@ -23180,7 +23180,7 @@
       </c>
       <c r="R418" s="3"/>
     </row>
-    <row r="419" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A419">
         <v>463</v>
       </c>
@@ -23231,7 +23231,7 @@
       </c>
       <c r="R419" s="3"/>
     </row>
-    <row r="420" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A420">
         <v>464</v>
       </c>
@@ -23282,7 +23282,7 @@
       </c>
       <c r="R420" s="3"/>
     </row>
-    <row r="421" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A421">
         <v>465</v>
       </c>
@@ -23333,7 +23333,7 @@
       </c>
       <c r="R421" s="3"/>
     </row>
-    <row r="422" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A422">
         <v>466</v>
       </c>
@@ -23384,7 +23384,7 @@
       </c>
       <c r="R422" s="3"/>
     </row>
-    <row r="423" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A423">
         <v>467</v>
       </c>
@@ -23435,7 +23435,7 @@
       </c>
       <c r="R423" s="3"/>
     </row>
-    <row r="424" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A424">
         <v>468</v>
       </c>
@@ -23486,7 +23486,7 @@
       </c>
       <c r="R424" s="3"/>
     </row>
-    <row r="425" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A425">
         <v>469</v>
       </c>
@@ -23537,7 +23537,7 @@
       </c>
       <c r="R425" s="3"/>
     </row>
-    <row r="426" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A426">
         <v>470</v>
       </c>
@@ -23588,7 +23588,7 @@
       </c>
       <c r="R426" s="3"/>
     </row>
-    <row r="427" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A427">
         <v>472</v>
       </c>
@@ -23599,7 +23599,7 @@
         <v>0</v>
       </c>
       <c r="D427">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="E427">
         <v>0</v>
@@ -23639,7 +23639,7 @@
       </c>
       <c r="R427" s="3"/>
     </row>
-    <row r="428" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A428">
         <v>473</v>
       </c>
@@ -23690,7 +23690,7 @@
       </c>
       <c r="R428" s="3"/>
     </row>
-    <row r="429" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A429">
         <v>474</v>
       </c>
@@ -23741,7 +23741,7 @@
       </c>
       <c r="R429" s="3"/>
     </row>
-    <row r="430" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A430">
         <v>475</v>
       </c>
@@ -23792,7 +23792,7 @@
       </c>
       <c r="R430" s="3"/>
     </row>
-    <row r="431" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A431">
         <v>476</v>
       </c>
@@ -23843,7 +23843,7 @@
       </c>
       <c r="R431" s="3"/>
     </row>
-    <row r="432" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A432">
         <v>477</v>
       </c>
@@ -23894,7 +23894,7 @@
       </c>
       <c r="R432" s="3"/>
     </row>
-    <row r="433" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A433">
         <v>478</v>
       </c>
@@ -23945,7 +23945,7 @@
       </c>
       <c r="R433" s="3"/>
     </row>
-    <row r="434" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A434">
         <v>479</v>
       </c>
@@ -23996,7 +23996,7 @@
       </c>
       <c r="R434" s="3"/>
     </row>
-    <row r="435" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A435">
         <v>480</v>
       </c>
@@ -24047,7 +24047,7 @@
       </c>
       <c r="R435" s="3"/>
     </row>
-    <row r="436" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A436">
         <v>481</v>
       </c>
@@ -24098,7 +24098,7 @@
       </c>
       <c r="R436" s="3"/>
     </row>
-    <row r="437" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A437">
         <v>482</v>
       </c>
@@ -24149,7 +24149,7 @@
       </c>
       <c r="R437" s="3"/>
     </row>
-    <row r="438" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A438">
         <v>483</v>
       </c>
@@ -24200,7 +24200,7 @@
       </c>
       <c r="R438" s="3"/>
     </row>
-    <row r="439" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A439">
         <v>484</v>
       </c>
@@ -24251,7 +24251,7 @@
       </c>
       <c r="R439" s="3"/>
     </row>
-    <row r="440" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A440">
         <v>485</v>
       </c>
@@ -24302,7 +24302,7 @@
       </c>
       <c r="R440" s="3"/>
     </row>
-    <row r="441" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A441">
         <v>486</v>
       </c>
@@ -24353,7 +24353,7 @@
       </c>
       <c r="R441" s="3"/>
     </row>
-    <row r="442" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A442">
         <v>487</v>
       </c>
@@ -24404,7 +24404,7 @@
       </c>
       <c r="R442" s="3"/>
     </row>
-    <row r="443" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A443">
         <v>488</v>
       </c>
@@ -24455,7 +24455,7 @@
       </c>
       <c r="R443" s="3"/>
     </row>
-    <row r="444" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A444">
         <v>489</v>
       </c>
@@ -24506,7 +24506,7 @@
       </c>
       <c r="R444" s="3"/>
     </row>
-    <row r="445" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A445">
         <v>490</v>
       </c>
@@ -24557,7 +24557,7 @@
       </c>
       <c r="R445" s="3"/>
     </row>
-    <row r="446" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A446">
         <v>491</v>
       </c>
@@ -24608,7 +24608,7 @@
       </c>
       <c r="R446" s="3"/>
     </row>
-    <row r="447" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A447">
         <v>492</v>
       </c>
@@ -24659,7 +24659,7 @@
       </c>
       <c r="R447" s="3"/>
     </row>
-    <row r="448" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A448">
         <v>493</v>
       </c>
@@ -24710,7 +24710,7 @@
       </c>
       <c r="R448" s="3"/>
     </row>
-    <row r="449" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A449">
         <v>494</v>
       </c>
@@ -24761,7 +24761,7 @@
       </c>
       <c r="R449" s="3"/>
     </row>
-    <row r="450" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A450">
         <v>495</v>
       </c>
@@ -24812,7 +24812,7 @@
       </c>
       <c r="R450" s="3"/>
     </row>
-    <row r="451" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A451">
         <v>496</v>
       </c>
@@ -24863,7 +24863,7 @@
       </c>
       <c r="R451" s="3"/>
     </row>
-    <row r="452" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A452">
         <v>497</v>
       </c>
@@ -24914,7 +24914,7 @@
       </c>
       <c r="R452" s="3"/>
     </row>
-    <row r="453" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A453">
         <v>498</v>
       </c>
@@ -24965,7 +24965,7 @@
       </c>
       <c r="R453" s="3"/>
     </row>
-    <row r="454" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A454">
         <v>499</v>
       </c>
@@ -25016,7 +25016,7 @@
       </c>
       <c r="R454" s="3"/>
     </row>
-    <row r="455" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A455">
         <v>500</v>
       </c>
@@ -25067,7 +25067,7 @@
       </c>
       <c r="R455" s="3"/>
     </row>
-    <row r="456" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A456">
         <v>501</v>
       </c>
@@ -25118,7 +25118,7 @@
       </c>
       <c r="R456" s="3"/>
     </row>
-    <row r="457" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A457">
         <v>502</v>
       </c>
@@ -25169,7 +25169,7 @@
       </c>
       <c r="R457" s="3"/>
     </row>
-    <row r="458" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A458">
         <v>503</v>
       </c>
@@ -25220,7 +25220,7 @@
       </c>
       <c r="R458" s="3"/>
     </row>
-    <row r="459" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A459">
         <v>504</v>
       </c>
@@ -25271,7 +25271,7 @@
       </c>
       <c r="R459" s="3"/>
     </row>
-    <row r="460" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A460">
         <v>505</v>
       </c>
@@ -25322,7 +25322,7 @@
       </c>
       <c r="R460" s="3"/>
     </row>
-    <row r="461" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A461">
         <v>506</v>
       </c>
@@ -25373,7 +25373,7 @@
       </c>
       <c r="R461" s="3"/>
     </row>
-    <row r="462" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A462">
         <v>507</v>
       </c>
@@ -25424,7 +25424,7 @@
       </c>
       <c r="R462" s="3"/>
     </row>
-    <row r="463" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A463">
         <v>508</v>
       </c>
@@ -25475,7 +25475,7 @@
       </c>
       <c r="R463" s="3"/>
     </row>
-    <row r="464" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A464">
         <v>509</v>
       </c>
@@ -25526,7 +25526,7 @@
       </c>
       <c r="R464" s="3"/>
     </row>
-    <row r="465" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A465">
         <v>510</v>
       </c>
@@ -25577,7 +25577,7 @@
       </c>
       <c r="R465" s="3"/>
     </row>
-    <row r="466" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A466">
         <v>511</v>
       </c>
@@ -25628,9 +25628,6 @@
       </c>
       <c r="R466" s="3"/>
     </row>
-    <row r="467" spans="1:18" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="468" spans="1:18" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="470" spans="1:18" ht="15" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Minor fix in PS column name
</commit_message>
<xml_diff>
--- a/official/L1Menu_Collisions2025_v1_1_1/PrescaleTable/L1Menu_Collisions2025_v1_1_1.xlsx
+++ b/official/L1Menu_Collisions2025_v1_1_1/PrescaleTable/L1Menu_Collisions2025_v1_1_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/L1MenuRun3-May16/official/L1Menu_Collisions2025_v1_1_1/PrescaleTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/L1MenuRun3-master_May25/official/L1Menu_Collisions2025_v1_1_1/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E76930-02A6-2444-A831-DE759D90DBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB197C4C-6F7F-AA4A-8A7A-F15D1DCA92B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="760" windowWidth="27760" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1460,9 +1460,6 @@
     <t>1p85E34</t>
   </si>
   <si>
-    <t>2p0E34_NoCICADA</t>
-  </si>
-  <si>
     <t>Backup1</t>
   </si>
   <si>
@@ -1476,6 +1473,9 @@
   </si>
   <si>
     <t>L1_DoubleTau_Iso34_Iso26_er2p1_Jet70_RmOvlp_dR0p5</t>
+  </si>
+  <si>
+    <t>2p0E34_NoL1CICADA</t>
   </si>
 </sst>
 </file>
@@ -1855,7 +1855,7 @@
   <dimension ref="A1:R466"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1904,13 +1904,13 @@
         <v>8</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>476</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="19" x14ac:dyDescent="0.2">
@@ -14566,7 +14566,7 @@
         <v>276</v>
       </c>
       <c r="B250" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C250">
         <v>0</v>
@@ -14617,7 +14617,7 @@
         <v>277</v>
       </c>
       <c r="B251" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C251">
         <v>0</v>
@@ -14668,7 +14668,7 @@
         <v>278</v>
       </c>
       <c r="B252" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C252">
         <v>0</v>

</xml_diff>

<commit_message>
Enabling seed "L1_DoubleMu3er2p0_SQ_OS_dR_Max1p6" from 1p95
</commit_message>
<xml_diff>
--- a/official/L1Menu_Collisions2025_v1_1_1/PrescaleTable/L1Menu_Collisions2025_v1_1_1.xlsx
+++ b/official/L1Menu_Collisions2025_v1_1_1/PrescaleTable/L1Menu_Collisions2025_v1_1_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/L1MenuRun3-master_May25/official/L1Menu_Collisions2025_v1_1_1/PrescaleTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/L1MenuRun3-master_Jun3/official/L1Menu_Collisions2025_v1_1_1/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB197C4C-6F7F-AA4A-8A7A-F15D1DCA92B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBD3364-A115-574F-9D9D-33E774EDD036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="760" windowWidth="27760" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R466"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6217,7 +6217,7 @@
         <v>0</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H86">
         <v>1</v>

</xml_diff>

<commit_message>
Enabling CICADA Loose seed
</commit_message>
<xml_diff>
--- a/official/L1Menu_Collisions2025_v1_1_1/PrescaleTable/L1Menu_Collisions2025_v1_1_1.xlsx
+++ b/official/L1Menu_Collisions2025_v1_1_1/PrescaleTable/L1Menu_Collisions2025_v1_1_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/L1MenuRun3-master_Jun3/official/L1Menu_Collisions2025_v1_1_1/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBD3364-A115-574F-9D9D-33E774EDD036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8EE07D-85F5-5444-83FD-F93D1A151FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="760" windowWidth="27760" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R466"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="G87" sqref="G87"/>
+    <sheetView tabSelected="1" topLeftCell="A367" workbookViewId="0">
+      <selection activeCell="E383" sqref="E383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21508,31 +21508,31 @@
         <v>0</v>
       </c>
       <c r="D386">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E386">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F386">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G386">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H386">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I386">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J386">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K386">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L386">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M386">
         <v>0</v>
@@ -21541,10 +21541,10 @@
         <v>0</v>
       </c>
       <c r="O386">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P386">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R386" s="3"/>
     </row>

</xml_diff>